<commit_message>
A whole bunch of changes to stuff
</commit_message>
<xml_diff>
--- a/Testing/SensorServo Tests.xlsx
+++ b/Testing/SensorServo Tests.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant\Documents\GitHub\Yavin4DefenceSystem\Testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="4" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -290,6 +295,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -297,7 +305,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -324,7 +332,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -971,11 +978,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="90624768"/>
-        <c:axId val="90825856"/>
+        <c:axId val="200938176"/>
+        <c:axId val="200938568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90624768"/>
+        <c:axId val="200938176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,19 +1004,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90825856"/>
+        <c:crossAx val="200938568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90825856"/>
+        <c:axId val="200938568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,21 +1038,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90624768"/>
+        <c:crossAx val="200938176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1059,7 +1063,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1714,11 +1718,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="59208832"/>
-        <c:axId val="55916032"/>
+        <c:axId val="200939352"/>
+        <c:axId val="200939744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59208832"/>
+        <c:axId val="200939352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1728,12 +1732,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55916032"/>
+        <c:crossAx val="200939744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55916032"/>
+        <c:axId val="200939744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +1748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59208832"/>
+        <c:crossAx val="200939352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1769,7 +1773,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2424,11 +2428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="59133952"/>
-        <c:axId val="59135488"/>
+        <c:axId val="200940528"/>
+        <c:axId val="200940920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59133952"/>
+        <c:axId val="200940528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2438,12 +2442,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59135488"/>
+        <c:crossAx val="200940920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59135488"/>
+        <c:axId val="200940920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2454,7 +2458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59133952"/>
+        <c:crossAx val="200940528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2479,7 +2483,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2733,11 +2737,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="59270656"/>
-        <c:axId val="59139584"/>
+        <c:axId val="200941704"/>
+        <c:axId val="200942096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59270656"/>
+        <c:axId val="200941704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,12 +2777,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59139584"/>
+        <c:crossAx val="200942096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59139584"/>
+        <c:axId val="200942096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2809,7 +2813,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59270656"/>
+        <c:crossAx val="200941704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2834,7 +2838,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3098,11 +3102,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93328896"/>
-        <c:axId val="93327360"/>
+        <c:axId val="200942880"/>
+        <c:axId val="200943272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93328896"/>
+        <c:axId val="200942880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3118,12 +3122,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93327360"/>
+        <c:crossAx val="200943272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93327360"/>
+        <c:axId val="200943272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3139,7 +3143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93328896"/>
+        <c:crossAx val="200942880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3374,7 +3378,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3409,7 +3413,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3620,8 +3624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AM125"/>
   <sheetViews>
-    <sheetView topLeftCell="R46" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6203,7 +6207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>